<commit_message>
some model correction in Requirement page
</commit_message>
<xml_diff>
--- a/sample_csv/customer_requirements_data.xlsx
+++ b/sample_csv/customer_requirements_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/raghuvallikkat/Desktop/LEADSOC_CODE/CRM1.0/sample_csv/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36A56E4E-7D5E-FD44-9A59-22BEF852684E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D29B591-644C-5E40-B4C4-FDF2175A83CD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6720" yWindow="560" windowWidth="27480" windowHeight="8200" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1320" yWindow="560" windowWidth="27480" windowHeight="8200" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="26">
   <si>
     <t>Customer</t>
   </si>
@@ -81,9 +81,6 @@
     <t>Good work in the domain of software engineering with pytho automation</t>
   </si>
   <si>
-    <t>Non-Active</t>
-  </si>
-  <si>
     <t>Ashok</t>
   </si>
   <si>
@@ -93,7 +90,19 @@
     <t>Yahasan</t>
   </si>
   <si>
-    <t>Sandeep</t>
+    <t>history</t>
+  </si>
+  <si>
+    <t>priority</t>
+  </si>
+  <si>
+    <t>nw req</t>
+  </si>
+  <si>
+    <t>Sandeep P</t>
+  </si>
+  <si>
+    <t>Closed</t>
   </si>
 </sst>
 </file>
@@ -445,10 +454,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:L5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -462,7 +471,7 @@
     <col min="8" max="8" width="20.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -493,8 +502,14 @@
       <c r="J1" t="s">
         <v>9</v>
       </c>
+      <c r="K1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L1" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -520,13 +535,19 @@
         <v>13</v>
       </c>
       <c r="I2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J2" t="s">
         <v>14</v>
       </c>
+      <c r="K2" t="s">
+        <v>23</v>
+      </c>
+      <c r="L2">
+        <v>1</v>
+      </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -549,16 +570,22 @@
         <v>10</v>
       </c>
       <c r="H3" t="s">
+        <v>25</v>
+      </c>
+      <c r="I3" t="s">
+        <v>20</v>
+      </c>
+      <c r="J3" t="s">
         <v>18</v>
       </c>
-      <c r="I3" t="s">
-        <v>21</v>
-      </c>
-      <c r="J3" t="s">
-        <v>19</v>
+      <c r="K3" t="s">
+        <v>23</v>
+      </c>
+      <c r="L3">
+        <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -581,16 +608,22 @@
         <v>10</v>
       </c>
       <c r="H4" t="s">
+        <v>25</v>
+      </c>
+      <c r="I4" t="s">
+        <v>24</v>
+      </c>
+      <c r="J4" t="s">
         <v>18</v>
       </c>
-      <c r="I4" t="s">
-        <v>22</v>
-      </c>
-      <c r="J4" t="s">
-        <v>19</v>
+      <c r="K4" t="s">
+        <v>23</v>
+      </c>
+      <c r="L4">
+        <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -613,13 +646,19 @@
         <v>10</v>
       </c>
       <c r="H5" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="I5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J5" t="s">
         <v>14</v>
+      </c>
+      <c r="K5" t="s">
+        <v>23</v>
+      </c>
+      <c r="L5">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adding seqNo. to sales req sheet
</commit_message>
<xml_diff>
--- a/sample_csv/customer_requirements_data.xlsx
+++ b/sample_csv/customer_requirements_data.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/raghuvallikkat/Desktop/LEADSOC_CODE/CRM1.0/sample_csv/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABE1402E-11F8-A74F-AD99-C5895FE47069}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F92206DC-C2F1-2B46-AE54-2B21851201A5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="980" yWindow="500" windowWidth="27480" windowHeight="17440" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="181029" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="47">
   <si>
     <t>Customer</t>
   </si>
@@ -163,6 +163,9 @@
   </si>
   <si>
     <t>Nayeem</t>
+  </si>
+  <si>
+    <t>SlNo</t>
   </si>
 </sst>
 </file>
@@ -515,349 +518,364 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:U5"/>
+  <dimension ref="A1:V5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.83203125" customWidth="1"/>
-    <col min="4" max="4" width="12.5" customWidth="1"/>
-    <col min="5" max="5" width="13.5" customWidth="1"/>
-    <col min="6" max="6" width="12.5" customWidth="1"/>
-    <col min="7" max="7" width="13.5" customWidth="1"/>
-    <col min="8" max="8" width="10.6640625" customWidth="1"/>
-    <col min="9" max="9" width="13.1640625" customWidth="1"/>
-    <col min="10" max="10" width="6.33203125" customWidth="1"/>
-    <col min="13" max="13" width="12.5" customWidth="1"/>
-    <col min="14" max="14" width="12.83203125" customWidth="1"/>
-    <col min="15" max="15" width="19.1640625" customWidth="1"/>
-    <col min="20" max="20" width="14.83203125" customWidth="1"/>
-    <col min="21" max="21" width="21.83203125" customWidth="1"/>
+    <col min="3" max="3" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.83203125" customWidth="1"/>
+    <col min="5" max="5" width="12.5" customWidth="1"/>
+    <col min="6" max="6" width="13.5" customWidth="1"/>
+    <col min="7" max="7" width="12.5" customWidth="1"/>
+    <col min="8" max="8" width="13.5" customWidth="1"/>
+    <col min="9" max="9" width="10.6640625" customWidth="1"/>
+    <col min="10" max="10" width="13.1640625" customWidth="1"/>
+    <col min="11" max="11" width="6.33203125" customWidth="1"/>
+    <col min="14" max="14" width="12.5" customWidth="1"/>
+    <col min="15" max="15" width="12.83203125" customWidth="1"/>
+    <col min="16" max="16" width="19.1640625" customWidth="1"/>
+    <col min="21" max="21" width="14.83203125" customWidth="1"/>
+    <col min="22" max="22" width="21.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B1" t="s">
         <v>23</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>30</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
-        <v>2</v>
-      </c>
       <c r="G1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" t="s">
         <v>24</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>25</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>4</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>27</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>26</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>5</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>37</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>38</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>6</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>7</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>28</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>19</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>29</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>41</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A2" s="1">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>10000</v>
+      </c>
+      <c r="B2" s="1">
         <v>45026</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>8</v>
       </c>
-      <c r="C2">
-        <v>2</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="D2">
+        <v>2</v>
+      </c>
+      <c r="E2" t="s">
         <v>31</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>10</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>9</v>
       </c>
-      <c r="G2">
-        <v>2</v>
-      </c>
       <c r="H2">
+        <v>2</v>
+      </c>
+      <c r="I2">
         <v>4</v>
       </c>
-      <c r="I2">
+      <c r="J2">
         <v>6</v>
       </c>
-      <c r="J2">
+      <c r="K2">
         <v>3</v>
       </c>
-      <c r="K2">
+      <c r="L2">
         <v>1</v>
       </c>
-      <c r="L2">
-        <v>2</v>
-      </c>
-      <c r="M2" t="s">
+      <c r="M2">
+        <v>2</v>
+      </c>
+      <c r="N2" t="s">
         <v>11</v>
       </c>
-      <c r="O2" t="s">
+      <c r="P2" t="s">
         <v>17</v>
       </c>
-      <c r="P2" t="s">
+      <c r="Q2" t="s">
         <v>12</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="R2" t="s">
         <v>20</v>
       </c>
-      <c r="R2">
+      <c r="S2">
         <v>1</v>
       </c>
-      <c r="S2" t="s">
+      <c r="T2" t="s">
         <v>35</v>
       </c>
-      <c r="T2">
-        <v>2</v>
-      </c>
-      <c r="U2" t="s">
+      <c r="U2">
+        <v>2</v>
+      </c>
+      <c r="V2" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A3" s="1">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>10001</v>
+      </c>
+      <c r="B3" s="1">
         <v>45026</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>13</v>
       </c>
-      <c r="C3">
+      <c r="D3">
         <v>3</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>32</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>15</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>14</v>
       </c>
-      <c r="G3">
+      <c r="H3">
         <v>4</v>
       </c>
-      <c r="H3">
+      <c r="I3">
         <v>6</v>
       </c>
-      <c r="I3">
+      <c r="J3">
         <v>10</v>
       </c>
-      <c r="J3">
+      <c r="K3">
         <v>6</v>
       </c>
-      <c r="K3">
-        <v>2</v>
-      </c>
       <c r="L3">
         <v>2</v>
       </c>
-      <c r="M3" t="s">
+      <c r="M3">
+        <v>2</v>
+      </c>
+      <c r="N3" t="s">
         <v>39</v>
       </c>
-      <c r="N3" s="1">
+      <c r="O3" s="1">
         <v>45056</v>
       </c>
-      <c r="O3" t="s">
+      <c r="P3" t="s">
         <v>18</v>
       </c>
-      <c r="P3" t="s">
+      <c r="Q3" t="s">
         <v>16</v>
       </c>
-      <c r="Q3" t="s">
+      <c r="R3" t="s">
         <v>20</v>
       </c>
-      <c r="R3">
-        <v>2</v>
-      </c>
-      <c r="S3" t="s">
+      <c r="S3">
+        <v>2</v>
+      </c>
+      <c r="T3" t="s">
         <v>36</v>
       </c>
-      <c r="T3">
+      <c r="U3">
         <v>3</v>
       </c>
-      <c r="U3" t="s">
+      <c r="V3" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A4" s="1">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>10002</v>
+      </c>
+      <c r="B4" s="1">
         <v>45026</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>13</v>
       </c>
-      <c r="C4">
+      <c r="D4">
         <v>4</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>33</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>15</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>14</v>
       </c>
-      <c r="G4">
+      <c r="H4">
         <v>8</v>
-      </c>
-      <c r="H4">
-        <v>10</v>
       </c>
       <c r="I4">
         <v>10</v>
       </c>
       <c r="J4">
+        <v>10</v>
+      </c>
+      <c r="K4">
         <v>6</v>
       </c>
-      <c r="K4">
-        <v>2</v>
-      </c>
       <c r="L4">
         <v>2</v>
       </c>
-      <c r="M4" t="s">
+      <c r="M4">
+        <v>2</v>
+      </c>
+      <c r="N4" t="s">
         <v>22</v>
       </c>
-      <c r="N4" s="1">
+      <c r="O4" s="1">
         <v>45056</v>
       </c>
-      <c r="O4" t="s">
+      <c r="P4" t="s">
         <v>21</v>
       </c>
-      <c r="P4" t="s">
+      <c r="Q4" t="s">
         <v>16</v>
       </c>
-      <c r="Q4" t="s">
+      <c r="R4" t="s">
         <v>20</v>
       </c>
-      <c r="R4">
+      <c r="S4">
         <v>3</v>
       </c>
-      <c r="S4" t="s">
+      <c r="T4" t="s">
         <v>40</v>
       </c>
-      <c r="T4">
+      <c r="U4">
         <v>1</v>
       </c>
-      <c r="U4" t="s">
+      <c r="V4" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A5" s="1">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>10003</v>
+      </c>
+      <c r="B5" s="1">
         <v>45026</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>13</v>
       </c>
-      <c r="C5">
+      <c r="D5">
         <v>5</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>34</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>15</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>14</v>
       </c>
-      <c r="G5">
-        <v>2</v>
-      </c>
       <c r="H5">
+        <v>2</v>
+      </c>
+      <c r="I5">
         <v>4</v>
       </c>
-      <c r="I5">
+      <c r="J5">
         <v>10</v>
       </c>
-      <c r="J5">
+      <c r="K5">
         <v>6</v>
       </c>
-      <c r="K5">
+      <c r="L5">
         <v>4</v>
       </c>
-      <c r="L5">
+      <c r="M5">
         <v>0</v>
       </c>
-      <c r="M5" t="s">
+      <c r="N5" t="s">
         <v>22</v>
       </c>
-      <c r="N5" s="1">
+      <c r="O5" s="1">
         <v>45056</v>
       </c>
-      <c r="O5" t="s">
+      <c r="P5" t="s">
         <v>18</v>
       </c>
-      <c r="P5" t="s">
+      <c r="Q5" t="s">
         <v>12</v>
       </c>
-      <c r="Q5" t="s">
+      <c r="R5" t="s">
         <v>20</v>
       </c>
-      <c r="R5">
+      <c r="S5">
         <v>1</v>
       </c>
-      <c r="S5" t="s">
+      <c r="T5" t="s">
         <v>35</v>
       </c>
-      <c r="T5">
+      <c r="U5">
         <v>3</v>
       </c>
-      <c r="U5" t="s">
+      <c r="V5" t="s">
         <v>44</v>
       </c>
     </row>

</xml_diff>